<commit_message>
add Crisis and Credit Allocation
</commit_message>
<xml_diff>
--- a/MappingTheFederalReserve'sResponseFunctionWithDirectedAcyclicGraphs/A Diff-in-DiffDAGOLS 2006-12-31 to 2008-09-30 parallel0.2.xlsx
+++ b/MappingTheFederalReserve'sResponseFunctionWithDirectedAcyclicGraphs/A Diff-in-DiffDAGOLS 2006-12-31 to 2008-09-30 parallel0.2.xlsx
@@ -19,7 +19,7 @@
     <t>A</t>
   </si>
   <si>
-    <t>LF</t>
+    <t>V</t>
   </si>
   <si>
     <t>Source</t>
@@ -28,19 +28,19 @@
     <t>A Lag</t>
   </si>
   <si>
-    <t>LF Lag</t>
-  </si>
-  <si>
-    <t>-0.021</t>
-  </si>
-  <si>
-    <t>-0.013</t>
-  </si>
-  <si>
-    <t>-3.442</t>
-  </si>
-  <si>
-    <t>1.049***</t>
+    <t>V Lag</t>
+  </si>
+  <si>
+    <t>-0.04</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>5.81</t>
+  </si>
+  <si>
+    <t>-1.11***</t>
   </si>
 </sst>
 </file>

</xml_diff>